<commit_message>
developer edition by default for 2016 + error handling
</commit_message>
<xml_diff>
--- a/sqlserver2016/docs/sql2016_ParamGenerator.xlsx
+++ b/sqlserver2016/docs/sql2016_ParamGenerator.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="596">
   <si>
     <t>https://msdn.microsoft.com/en-us/library/ms144259.aspx?f=255&amp;MSPPError=-2147217396</t>
   </si>
@@ -2323,6 +2323,9 @@
   </si>
   <si>
     <t>MSSQLSERVER</t>
+  </si>
+  <si>
+    <t>22222-00000-00000-00000-00000</t>
   </si>
 </sst>
 </file>
@@ -2739,8 +2742,8 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3653,7 +3656,9 @@
       <c r="F25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="2"/>
+      <c r="G25" t="s">
+        <v>595</v>
+      </c>
       <c r="J25" t="str">
         <f t="shared" si="5"/>
         <v>choco:sqlserver2016:PID</v>
@@ -3662,11 +3667,11 @@
         <v>1</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>if (!(Test-Path env:\choco:sqlserver2016:PID)){$env:choco:sqlserver2016:PID="22222-00000-00000-00000-00000"}</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="7"/>
@@ -8577,87 +8582,25 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="A347:A349"/>
-    <mergeCell ref="C347:C349"/>
-    <mergeCell ref="A318:A322"/>
-    <mergeCell ref="A323:A327"/>
-    <mergeCell ref="A328:A340"/>
-    <mergeCell ref="A341:A343"/>
-    <mergeCell ref="C341:C343"/>
-    <mergeCell ref="A344:A346"/>
-    <mergeCell ref="C344:C346"/>
-    <mergeCell ref="A306:A308"/>
-    <mergeCell ref="A309:A311"/>
-    <mergeCell ref="A312:A314"/>
-    <mergeCell ref="C312:C314"/>
-    <mergeCell ref="A315:A317"/>
-    <mergeCell ref="C315:C317"/>
-    <mergeCell ref="A279:A283"/>
-    <mergeCell ref="A284:A286"/>
-    <mergeCell ref="A287:A295"/>
-    <mergeCell ref="A296:A300"/>
-    <mergeCell ref="C296:C300"/>
-    <mergeCell ref="A301:A305"/>
-    <mergeCell ref="A247:A255"/>
-    <mergeCell ref="A256:A262"/>
-    <mergeCell ref="A263:A265"/>
-    <mergeCell ref="A266:A272"/>
-    <mergeCell ref="A273:A275"/>
-    <mergeCell ref="A276:A278"/>
-    <mergeCell ref="A224:A226"/>
-    <mergeCell ref="C224:C226"/>
-    <mergeCell ref="A227:A233"/>
-    <mergeCell ref="A234:A236"/>
-    <mergeCell ref="A237:A241"/>
-    <mergeCell ref="A242:A246"/>
-    <mergeCell ref="A203:A207"/>
-    <mergeCell ref="A208:A210"/>
-    <mergeCell ref="A211:A213"/>
-    <mergeCell ref="A214:A220"/>
-    <mergeCell ref="A221:A223"/>
-    <mergeCell ref="C221:C223"/>
-    <mergeCell ref="A185:A191"/>
-    <mergeCell ref="A192:A194"/>
-    <mergeCell ref="C192:C194"/>
-    <mergeCell ref="A195:A199"/>
-    <mergeCell ref="A200:A202"/>
-    <mergeCell ref="C200:C202"/>
-    <mergeCell ref="A170:A172"/>
-    <mergeCell ref="A173:A175"/>
-    <mergeCell ref="A176:A178"/>
-    <mergeCell ref="C176:C178"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A182:A184"/>
-    <mergeCell ref="A152:A154"/>
-    <mergeCell ref="C152:C154"/>
-    <mergeCell ref="A155:A161"/>
-    <mergeCell ref="A162:A164"/>
-    <mergeCell ref="C162:C164"/>
-    <mergeCell ref="A165:A169"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A145"/>
-    <mergeCell ref="A146:A148"/>
-    <mergeCell ref="C146:C148"/>
-    <mergeCell ref="A149:A151"/>
-    <mergeCell ref="C149:C151"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="C111:C113"/>
-    <mergeCell ref="A114:A122"/>
-    <mergeCell ref="A123:A127"/>
-    <mergeCell ref="A128:A130"/>
-    <mergeCell ref="A131:A135"/>
-    <mergeCell ref="A85:A95"/>
-    <mergeCell ref="A96:A104"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="C105:C107"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="C108:C110"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="A64:A66"/>
     <mergeCell ref="C64:C66"/>
     <mergeCell ref="A67:A69"/>
@@ -8672,25 +8615,87 @@
     <mergeCell ref="A58:A60"/>
     <mergeCell ref="A61:A63"/>
     <mergeCell ref="C61:C63"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A85:A95"/>
+    <mergeCell ref="A96:A104"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="C105:C107"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="C108:C110"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A145"/>
+    <mergeCell ref="A146:A148"/>
+    <mergeCell ref="C146:C148"/>
+    <mergeCell ref="A149:A151"/>
+    <mergeCell ref="C149:C151"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="C111:C113"/>
+    <mergeCell ref="A114:A122"/>
+    <mergeCell ref="A123:A127"/>
+    <mergeCell ref="A128:A130"/>
+    <mergeCell ref="A131:A135"/>
+    <mergeCell ref="A170:A172"/>
+    <mergeCell ref="A173:A175"/>
+    <mergeCell ref="A176:A178"/>
+    <mergeCell ref="C176:C178"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A184"/>
+    <mergeCell ref="A152:A154"/>
+    <mergeCell ref="C152:C154"/>
+    <mergeCell ref="A155:A161"/>
+    <mergeCell ref="A162:A164"/>
+    <mergeCell ref="C162:C164"/>
+    <mergeCell ref="A165:A169"/>
+    <mergeCell ref="A203:A207"/>
+    <mergeCell ref="A208:A210"/>
+    <mergeCell ref="A211:A213"/>
+    <mergeCell ref="A214:A220"/>
+    <mergeCell ref="A221:A223"/>
+    <mergeCell ref="C221:C223"/>
+    <mergeCell ref="A185:A191"/>
+    <mergeCell ref="A192:A194"/>
+    <mergeCell ref="C192:C194"/>
+    <mergeCell ref="A195:A199"/>
+    <mergeCell ref="A200:A202"/>
+    <mergeCell ref="C200:C202"/>
+    <mergeCell ref="A247:A255"/>
+    <mergeCell ref="A256:A262"/>
+    <mergeCell ref="A263:A265"/>
+    <mergeCell ref="A266:A272"/>
+    <mergeCell ref="A273:A275"/>
+    <mergeCell ref="A276:A278"/>
+    <mergeCell ref="A224:A226"/>
+    <mergeCell ref="C224:C226"/>
+    <mergeCell ref="A227:A233"/>
+    <mergeCell ref="A234:A236"/>
+    <mergeCell ref="A237:A241"/>
+    <mergeCell ref="A242:A246"/>
+    <mergeCell ref="A306:A308"/>
+    <mergeCell ref="A309:A311"/>
+    <mergeCell ref="A312:A314"/>
+    <mergeCell ref="C312:C314"/>
+    <mergeCell ref="A315:A317"/>
+    <mergeCell ref="C315:C317"/>
+    <mergeCell ref="A279:A283"/>
+    <mergeCell ref="A284:A286"/>
+    <mergeCell ref="A287:A295"/>
+    <mergeCell ref="A296:A300"/>
+    <mergeCell ref="C296:C300"/>
+    <mergeCell ref="A301:A305"/>
+    <mergeCell ref="A347:A349"/>
+    <mergeCell ref="C347:C349"/>
+    <mergeCell ref="A318:A322"/>
+    <mergeCell ref="A323:A327"/>
+    <mergeCell ref="A328:A340"/>
+    <mergeCell ref="A341:A343"/>
+    <mergeCell ref="C341:C343"/>
+    <mergeCell ref="A344:A346"/>
+    <mergeCell ref="C344:C346"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C17" r:id="rId1" display="https://msdn.microsoft.com/en-us/library/dd239405.aspx"/>

</xml_diff>